<commit_message>
Fixing schema: pattern for study accession was wrong.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4078039-53F9-2947-AB1B-5AB3E2D2C724}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0983DEED-3B5D-634A-8144-090D039448DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -475,9 +475,6 @@
     <t>Linking associations with study. Must match the study tag in the study table</t>
   </si>
   <si>
-    <t>^GCST\d+*$</t>
-  </si>
-  <si>
     <t>GCST007280</t>
   </si>
   <si>
@@ -548,6 +545,9 @@
   </si>
   <si>
     <t>Stage of the experimental design</t>
+  </si>
+  <si>
+    <t>^GCST\d+$</t>
   </si>
 </sst>
 </file>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -994,10 +994,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -1049,11 +1049,11 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="C3" s="5" t="b">
         <v>0</v>
       </c>
@@ -1070,13 +1070,13 @@
         <v>24</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1301,7 +1301,7 @@
         <v>54</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1309,25 +1309,25 @@
         <v>88</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="C12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1422,7 +1422,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>62</v>
@@ -1474,7 +1474,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -1500,60 +1500,60 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="L19" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1604,10 +1604,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>
@@ -1779,7 +1779,7 @@
         <v>24</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N6" s="5" t="b">
         <v>1</v>
@@ -1837,7 +1837,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>127</v>
@@ -1866,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>124</v>
@@ -2065,7 +2065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2101,10 +2101,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>3</v>
@@ -2165,7 +2165,7 @@
         <v>100</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C3" s="7" t="b">
         <v>1</v>
@@ -2374,7 +2374,7 @@
         <v>24</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3439,10 +3439,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updating schema: making study tag mandatory in the notes tab.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0983DEED-3B5D-634A-8144-090D039448DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFFEDF0-43B6-A043-83C5-904A788A3823}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="35500" yWindow="-3320" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -960,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -3405,8 +3405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4CB50-F135-6F43-A6BC-AC27D4D7EACE}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3504,7 +3504,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="7" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
making ancestry column default for all users.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1538674-D3A7-F541-B488-E839D16A07B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71616C4A-619B-AA41-A35A-7192C8F969E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35500" yWindow="-3320" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="38260" yWindow="1140" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -2065,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2333,7 +2333,7 @@
         <v>79</v>
       </c>
       <c r="C9" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="7" t="b">
         <v>0</v>
@@ -3405,7 +3405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4CB50-F135-6F43-A6BC-AC27D4D7EACE}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+    <sheetView zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
A new column ('Readme file') is added to the study spreadsheet. It's optional in all cases.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71616C4A-619B-AA41-A35A-7192C8F969E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AD9FFC-B1DA-7F4B-9728-844F85EE7D2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38260" yWindow="1140" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="28800" yWindow="-2780" windowWidth="51160" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">association!$C$1:$C$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">study!$C$1:$C$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">study!$C$1:$C$19</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="173">
   <si>
     <t>NAME</t>
   </si>
@@ -548,6 +548,15 @@
   </si>
   <si>
     <t>^GCST\d+$</t>
+  </si>
+  <si>
+    <t>readme_file</t>
+  </si>
+  <si>
+    <t>Readme file</t>
+  </si>
+  <si>
+    <t>Path or URL pointing to the file containing additional information for the provided summary statistics file</t>
   </si>
 </sst>
 </file>
@@ -958,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1471,10 +1480,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>51</v>
+        <v>170</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="C18" s="5" t="b">
         <v>1</v>
@@ -1486,24 +1495,21 @@
         <v>0</v>
       </c>
       <c r="F18" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="L18" s="5" t="s">
-        <v>53</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>151</v>
+        <v>51</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C19" s="5" t="b">
         <v>1</v>
@@ -1515,44 +1521,73 @@
         <v>0</v>
       </c>
       <c r="F19" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="5" t="s">
+      <c r="C21" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1567,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2065,7 +2100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
In the association sheet the effect and other allele now accept '-' representing deletions.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AD9FFC-B1DA-7F4B-9728-844F85EE7D2E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC970E4-2DA4-6143-976A-EC96520DC5E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-2780" windowWidth="51160" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="28800" yWindow="-2780" windowWidth="51160" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -541,9 +541,6 @@
     <t>checksum</t>
   </si>
   <si>
-    <t>^[actgACTG?]*$</t>
-  </si>
-  <si>
     <t>Stage of the experimental design</t>
   </si>
   <si>
@@ -557,6 +554,9 @@
   </si>
   <si>
     <t>Path or URL pointing to the file containing additional information for the provided summary statistics file</t>
+  </si>
+  <si>
+    <t>^[actgACTG?-]*$</t>
   </si>
 </sst>
 </file>
@@ -969,7 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1079,7 +1079,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>145</v>
@@ -1480,28 +1480,28 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1602,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -1872,7 +1872,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>127</v>
@@ -1901,7 +1901,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>124</v>
@@ -2200,7 +2200,7 @@
         <v>100</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" s="7" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Study tag column is now added to the Summary stats template sheet.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC970E4-2DA4-6143-976A-EC96520DC5E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516B1D7B-B504-1541-8682-67185FDF485B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-2780" windowWidth="51160" windowHeight="17540" activeTab="1" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1602,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150BB387-D897-2449-8E3B-2908679801E7}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Setting study tag mandatory for Summary stats schema.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516B1D7B-B504-1541-8682-67185FDF485B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE85AAD-1D14-084E-8EB8-06C54CC4AFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
@@ -970,7 +970,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Updated schema.xlsx: accepted builds added, summary stats are now mandatory for everyone.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dsuveges/repositories/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE85AAD-1D14-084E-8EB8-06C54CC4AFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4576D16-B110-2644-962C-86ACB87F9E11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="31380" yWindow="-2100" windowWidth="44240" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="174">
   <si>
     <t>NAME</t>
   </si>
@@ -557,6 +557,9 @@
   </si>
   <si>
     <t>^[actgACTG?-]*$</t>
+  </si>
+  <si>
+    <t>GRCh38|GRCh37|NCBI36|NCBI35|NCBI34</t>
   </si>
 </sst>
 </file>
@@ -970,7 +973,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1440,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="5" t="b">
         <v>1</v>
@@ -1452,7 +1455,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>166</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="5" t="b">
         <v>1</v>
@@ -1478,7 +1481,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>169</v>
       </c>
@@ -1504,7 +1507,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5" t="b">
         <v>1</v>
@@ -1532,8 +1535,11 @@
       <c r="L19" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>151</v>
       </c>
@@ -1562,7 +1568,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>153</v>
       </c>

</xml_diff>

<commit_message>
Drop-down options are enabled for long lists as well using invisible sheet.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dsuveges/repositories/gwas-template-services/schema_definitions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4576D16-B110-2644-962C-86ACB87F9E11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DCAB93-965C-8B44-8001-6DF4002B8B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="-2100" windowWidth="44240" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="31380" yWindow="-2100" windowWidth="44240" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="179">
   <si>
     <t>NAME</t>
   </si>
@@ -560,6 +560,21 @@
   </si>
   <si>
     <t>GRCh38|GRCh37|NCBI36|NCBI35|NCBI34</t>
+  </si>
+  <si>
+    <t>Aboriginal Australian|African American or Afro-Caribbean|African unspecified|Asian unspecified|Central Asian|Circumpolar peoples|East Asian|European|Greater Middle Eastern (Middle Eastern, North African or Persian)|Hispanic or Latin American|Native American|NR|Oceanian|Other|Other admixed ancestry|South Asian|South East Asian|Sub-Saharan African</t>
+  </si>
+  <si>
+    <t>Initial extraction</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>discovery, replication</t>
+  </si>
+  <si>
+    <t>yes, no</t>
   </si>
 </sst>
 </file>
@@ -972,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="C1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1216,9 @@
       <c r="G7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="L7" s="5" t="s">
         <v>35</v>
       </c>
@@ -1609,7 +1626,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2106,8 +2123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2223,6 +2240,9 @@
       <c r="G3" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="I3" s="7" t="s">
+        <v>177</v>
+      </c>
       <c r="L3" s="7" t="s">
         <v>99</v>
       </c>
@@ -2364,6 +2384,9 @@
       </c>
       <c r="L8" s="7" t="s">
         <v>81</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3446,8 +3469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED4CB50-F135-6F43-A6BC-AC27D4D7EACE}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="D1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3577,7 +3600,9 @@
       <c r="G4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>175</v>
+      </c>
       <c r="L4" s="5" t="s">
         <v>68</v>
       </c>
@@ -3604,7 +3629,9 @@
       <c r="G5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="L5" s="5" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Allowing specifiying NA as genome version.
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DCAB93-965C-8B44-8001-6DF4002B8B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C820726-8D3D-FF49-A343-F01C3E6A2EA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="-2100" windowWidth="44240" windowHeight="17540" activeTab="2" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -559,9 +559,6 @@
     <t>^[actgACTG?-]*$</t>
   </si>
   <si>
-    <t>GRCh38|GRCh37|NCBI36|NCBI35|NCBI34</t>
-  </si>
-  <si>
     <t>Aboriginal Australian|African American or Afro-Caribbean|African unspecified|Asian unspecified|Central Asian|Circumpolar peoples|East Asian|European|Greater Middle Eastern (Middle Eastern, North African or Persian)|Hispanic or Latin American|Native American|NR|Oceanian|Other|Other admixed ancestry|South Asian|South East Asian|Sub-Saharan African</t>
   </si>
   <si>
@@ -575,6 +572,9 @@
   </si>
   <si>
     <t>yes, no</t>
+  </si>
+  <si>
+    <t>GRCh38|GRCh37|NCBI36|NCBI35|NCBI34|NA</t>
   </si>
 </sst>
 </file>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1217,7 +1217,7 @@
         <v>44</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>35</v>
@@ -1553,7 +1553,7 @@
         <v>53</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -2123,7 +2123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EEE6B5-99CE-7744-8022-5400F74ED3C6}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="121" zoomScaleNormal="121" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -2241,7 +2241,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>99</v>
@@ -2386,7 +2386,7 @@
         <v>81</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3601,7 +3601,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>68</v>
@@ -3630,7 +3630,7 @@
         <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
changing missing build from NA to NR
</commit_message>
<xml_diff>
--- a/schema_definitions/template_schema_v1.2.xlsx
+++ b/schema_definitions/template_schema_v1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuveges/Project/gwas-template-services/schema_definitions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C820726-8D3D-FF49-A343-F01C3E6A2EA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F85767-B5DD-9C40-B98E-1789A8BBA5C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
+    <workbookView xWindow="38600" yWindow="2280" windowWidth="28800" windowHeight="17540" xr2:uid="{ED582597-DC63-654C-87F3-6CB4F7FD90A0}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -574,7 +574,7 @@
     <t>yes, no</t>
   </si>
   <si>
-    <t>GRCh38|GRCh37|NCBI36|NCBI35|NCBI34|NA</t>
+    <t>GRCh38|GRCh37|NCBI36|NCBI35|NCBI34|NR</t>
   </si>
 </sst>
 </file>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F5AB58-2CE3-8246-A104-E60B298CD92A}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>